<commit_message>
updated test_hist folder withcode adjustments
</commit_message>
<xml_diff>
--- a/checks/test_hist/corpora_stats.xlsx
+++ b/checks/test_hist/corpora_stats.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>Sentences</t>
+  </si>
+  <si>
+    <t>Unique_nouns</t>
+  </si>
+  <si>
+    <t>Unique_verbs</t>
   </si>
   <si>
     <t>Nlen_freq</t>
@@ -401,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,96 +435,141 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2">
+        <v>409</v>
+      </c>
+      <c r="D2">
+        <v>734</v>
+      </c>
+      <c r="E2">
+        <v>782</v>
+      </c>
+      <c r="F2">
         <v>6.01344537815126</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>7.128169014084507</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>6.614441416893733</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>7.332480818414322</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>0.1710144927536232</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
+        <v>882</v>
+      </c>
+      <c r="D3">
+        <v>2068</v>
+      </c>
+      <c r="E3">
+        <v>1297</v>
+      </c>
+      <c r="F3">
         <v>4.952865378094269</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>5.229932677369239</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>5.336557059961315</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>5.422513492675405</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>6.884615384615385</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>4.745375700841009</v>
+        <v>31688</v>
       </c>
       <c r="D4">
-        <v>3.054370268410186</v>
+        <v>16698</v>
       </c>
       <c r="E4">
-        <v>6.042947833287331</v>
+        <v>10581</v>
       </c>
       <c r="F4">
-        <v>6.319444444444445</v>
+        <v>4.734268878037985</v>
       </c>
       <c r="G4">
-        <v>1.904328018223235</v>
+        <v>3.825290787898494</v>
+      </c>
+      <c r="H4">
+        <v>6.057312252964427</v>
+      </c>
+      <c r="I4">
+        <v>5.028447216709195</v>
+      </c>
+      <c r="J4">
+        <v>1.794319743472286</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5">
+        <v>6236</v>
+      </c>
+      <c r="D5">
+        <v>8243</v>
+      </c>
+      <c r="E5">
+        <v>7966</v>
+      </c>
+      <c r="F5">
         <v>8.307227702838736</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>8.814446411832101</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>8.912289215091592</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>9.575696711021843</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>0.3836942675159236</v>
       </c>
     </row>

</xml_diff>